<commit_message>
When it is not necesary to make a decision, it is necesary not to make a decision.
</commit_message>
<xml_diff>
--- a/output/results.xlsx
+++ b/output/results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="87">
   <si>
     <t>Location</t>
   </si>
@@ -28,9 +28,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Yices Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">Revere Beach </t>
@@ -331,8 +328,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -351,7 +350,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -359,6 +358,7 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -366,6 +366,7 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1462,10 +1463,10 @@
                   <c:v>83.390384</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>0.0</c:v>
+                  <c:v>200.762828</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>0.0</c:v>
+                  <c:v>201.178559</c:v>
                 </c:pt>
                 <c:pt idx="149">
                   <c:v>83.54538599999999</c:v>
@@ -2689,10 +2690,10 @@
                   <c:v>7.07463</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>200.762828</c:v>
+                  <c:v>17.15869</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>201.178559</c:v>
+                  <c:v>17.142101</c:v>
                 </c:pt>
                 <c:pt idx="149">
                   <c:v>7.109068</c:v>
@@ -3268,10 +3269,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D200"/>
+  <dimension ref="A1:C200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="H146" sqref="H146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3289,7 +3290,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2">
         <v>277.36238600000001</v>
@@ -3300,7 +3301,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>310.65714400000002</v>
@@ -3311,7 +3312,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>342.154518</v>
@@ -3322,7 +3323,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>224.72029699999999</v>
@@ -3333,7 +3334,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>235.793171</v>
@@ -3344,7 +3345,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>249.11477400000001</v>
@@ -3355,7 +3356,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>108.18054100000001</v>
@@ -3366,7 +3367,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>0.90270600000000001</v>
@@ -3377,7 +3378,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>240.38934499999999</v>
@@ -3388,7 +3389,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>318.61999400000002</v>
@@ -3399,7 +3400,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>247.05590000000001</v>
@@ -3410,7 +3411,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B13">
         <v>237.119338</v>
@@ -3421,7 +3422,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B14">
         <v>261.36826200000002</v>
@@ -3432,7 +3433,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15">
         <v>257.98060400000003</v>
@@ -3443,7 +3444,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16">
         <v>272.85749499999997</v>
@@ -3454,7 +3455,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17">
         <v>286.47512</v>
@@ -3465,7 +3466,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18">
         <v>1.0283990000000001</v>
@@ -3476,7 +3477,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B19">
         <v>131.625047</v>
@@ -3487,7 +3488,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20">
         <v>281.89048400000001</v>
@@ -3498,7 +3499,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21">
         <v>306.00625000000002</v>
@@ -3509,7 +3510,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B22">
         <v>295.17156299999999</v>
@@ -3520,7 +3521,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B23">
         <v>363.46554200000003</v>
@@ -3531,7 +3532,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B24">
         <v>363.13314300000002</v>
@@ -3542,7 +3543,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B25">
         <v>313.94678099999999</v>
@@ -3553,7 +3554,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B26">
         <v>105.65446900000001</v>
@@ -3564,7 +3565,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B27">
         <v>125.395528</v>
@@ -3575,7 +3576,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B28">
         <v>124.34156400000001</v>
@@ -3586,7 +3587,7 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B29">
         <v>324.65819099999999</v>
@@ -3597,7 +3598,7 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B30">
         <v>342.323622</v>
@@ -3608,7 +3609,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B31">
         <v>300.858746</v>
@@ -3619,7 +3620,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B32">
         <v>328.99943400000001</v>
@@ -3630,7 +3631,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B33">
         <v>9.2456479999999992</v>
@@ -3641,7 +3642,7 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B34">
         <v>10.761366000000001</v>
@@ -3652,7 +3653,7 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B35">
         <v>351.15322300000003</v>
@@ -3663,7 +3664,7 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B36">
         <v>326.13991600000003</v>
@@ -3674,7 +3675,7 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B37">
         <v>306.62102499999997</v>
@@ -3685,7 +3686,7 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B38">
         <v>357.61619100000001</v>
@@ -3696,7 +3697,7 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B39">
         <v>123.91192700000001</v>
@@ -3707,7 +3708,7 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B40">
         <v>123.62097</v>
@@ -3718,7 +3719,7 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B41">
         <v>140.108891</v>
@@ -3729,7 +3730,7 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B42">
         <v>361.84411699999998</v>
@@ -3740,7 +3741,7 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B43">
         <v>356.12187</v>
@@ -3751,7 +3752,7 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B44">
         <v>297.920658</v>
@@ -3762,7 +3763,7 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B45">
         <v>500</v>
@@ -3773,7 +3774,7 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B46">
         <v>286.46579000000003</v>
@@ -3784,7 +3785,7 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B47">
         <v>15.73701</v>
@@ -3795,7 +3796,7 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B48">
         <v>18.726925000000001</v>
@@ -3806,7 +3807,7 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B49">
         <v>40.606903000000003</v>
@@ -3817,7 +3818,7 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B50">
         <v>35.267614999999999</v>
@@ -3828,7 +3829,7 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B51">
         <v>284.44006400000001</v>
@@ -3839,7 +3840,7 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B52">
         <v>0.428448</v>
@@ -3850,7 +3851,7 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B53">
         <v>30.213096</v>
@@ -3861,7 +3862,7 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B54">
         <v>30.438621999999999</v>
@@ -3872,7 +3873,7 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B55">
         <v>252.49244899999999</v>
@@ -3883,7 +3884,7 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B56">
         <v>292.10528499999998</v>
@@ -3894,7 +3895,7 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B57">
         <v>291.05469199999999</v>
@@ -3905,7 +3906,7 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B58">
         <v>298.19789600000001</v>
@@ -3916,7 +3917,7 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B59">
         <v>206.79555400000001</v>
@@ -3927,7 +3928,7 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B60">
         <v>197.544996</v>
@@ -3938,7 +3939,7 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B61">
         <v>94.879814999999994</v>
@@ -3949,7 +3950,7 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B62">
         <v>94.554880999999995</v>
@@ -3960,7 +3961,7 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B63">
         <v>197.62942200000001</v>
@@ -3971,7 +3972,7 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B64">
         <v>207.57945699999999</v>
@@ -3982,7 +3983,7 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B65">
         <v>315.26392099999998</v>
@@ -3993,7 +3994,7 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B66">
         <v>324.79168600000003</v>
@@ -4004,7 +4005,7 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B67">
         <v>330.62145099999998</v>
@@ -4015,7 +4016,7 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B68">
         <v>500</v>
@@ -4026,7 +4027,7 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B69">
         <v>107.794354</v>
@@ -4037,7 +4038,7 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B70">
         <v>125.44611999999999</v>
@@ -4048,7 +4049,7 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B71">
         <v>1.6122289999999999</v>
@@ -4059,7 +4060,7 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B72">
         <v>500</v>
@@ -4070,7 +4071,7 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B73">
         <v>93.596909999999994</v>
@@ -4081,7 +4082,7 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B74">
         <v>93.877784000000005</v>
@@ -4092,7 +4093,7 @@
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B75">
         <v>28.901790999999999</v>
@@ -4103,7 +4104,7 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B76">
         <v>30.182303999999998</v>
@@ -4114,7 +4115,7 @@
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B77">
         <v>500</v>
@@ -4125,7 +4126,7 @@
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B78">
         <v>500</v>
@@ -4136,7 +4137,7 @@
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B79">
         <v>500</v>
@@ -4147,7 +4148,7 @@
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B80">
         <v>446.503378</v>
@@ -4158,7 +4159,7 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B81">
         <v>382.66281300000003</v>
@@ -4169,7 +4170,7 @@
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B82">
         <v>379.28956499999998</v>
@@ -4180,7 +4181,7 @@
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B83">
         <v>328.43552099999999</v>
@@ -4191,7 +4192,7 @@
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B84">
         <v>320.27928200000002</v>
@@ -4202,7 +4203,7 @@
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B85">
         <v>255.36988400000001</v>
@@ -4213,7 +4214,7 @@
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B86">
         <v>260.82297599999998</v>
@@ -4224,7 +4225,7 @@
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B87">
         <v>11.338742</v>
@@ -4235,7 +4236,7 @@
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B88">
         <v>11.586138999999999</v>
@@ -4246,7 +4247,7 @@
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B89">
         <v>38.302008999999998</v>
@@ -4257,7 +4258,7 @@
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B90">
         <v>36.235187000000003</v>
@@ -4268,7 +4269,7 @@
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B91">
         <v>217.26123799999999</v>
@@ -4279,7 +4280,7 @@
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B92">
         <v>42.722293000000001</v>
@@ -4290,7 +4291,7 @@
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B93">
         <v>329.41551399999997</v>
@@ -4301,7 +4302,7 @@
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B94">
         <v>336.78127000000001</v>
@@ -4312,7 +4313,7 @@
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B95">
         <v>321.085891</v>
@@ -4323,7 +4324,7 @@
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B96">
         <v>327.59795500000001</v>
@@ -4334,7 +4335,7 @@
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B97">
         <v>316.80489899999998</v>
@@ -4345,7 +4346,7 @@
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B98">
         <v>330.22482000000002</v>
@@ -4356,7 +4357,7 @@
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B99">
         <v>333.77572800000002</v>
@@ -4367,7 +4368,7 @@
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B100">
         <v>500</v>
@@ -4378,7 +4379,7 @@
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B101">
         <v>296.49590899999998</v>
@@ -4389,7 +4390,7 @@
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B102">
         <v>315.52759099999997</v>
@@ -4400,7 +4401,7 @@
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B103">
         <v>295.00489299999998</v>
@@ -4411,7 +4412,7 @@
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B104">
         <v>294.533388</v>
@@ -4422,7 +4423,7 @@
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B105">
         <v>274.47617300000002</v>
@@ -4433,7 +4434,7 @@
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B106">
         <v>284.52989500000001</v>
@@ -4444,7 +4445,7 @@
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B107">
         <v>321.63242000000002</v>
@@ -4455,7 +4456,7 @@
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B108">
         <v>312.56026600000001</v>
@@ -4466,7 +4467,7 @@
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B109">
         <v>284.382274</v>
@@ -4477,7 +4478,7 @@
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B110">
         <v>286.94784700000002</v>
@@ -4488,7 +4489,7 @@
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B111">
         <v>287.92407400000002</v>
@@ -4499,7 +4500,7 @@
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B112">
         <v>500</v>
@@ -4510,7 +4511,7 @@
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B113">
         <v>328.17586899999998</v>
@@ -4521,7 +4522,7 @@
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B114">
         <v>309.951347</v>
@@ -4532,7 +4533,7 @@
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B115">
         <v>303.14842499999997</v>
@@ -4543,7 +4544,7 @@
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B116">
         <v>314.99758700000001</v>
@@ -4554,7 +4555,7 @@
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B117">
         <v>334.90690799999999</v>
@@ -4565,7 +4566,7 @@
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B118">
         <v>293.624165</v>
@@ -4576,7 +4577,7 @@
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B119">
         <v>37.679302</v>
@@ -4587,7 +4588,7 @@
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B120">
         <v>205.92843300000001</v>
@@ -4598,7 +4599,7 @@
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B121">
         <v>34.291313000000002</v>
@@ -4609,7 +4610,7 @@
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B122">
         <v>33.868704000000001</v>
@@ -4620,7 +4621,7 @@
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B123">
         <v>11.027654</v>
@@ -4631,7 +4632,7 @@
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B124">
         <v>11.020394</v>
@@ -4642,7 +4643,7 @@
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B125">
         <v>255.55402599999999</v>
@@ -4653,7 +4654,7 @@
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B126">
         <v>255.29410799999999</v>
@@ -4664,7 +4665,7 @@
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B127">
         <v>284.992773</v>
@@ -4675,7 +4676,7 @@
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B128">
         <v>285.86811599999999</v>
@@ -4686,7 +4687,7 @@
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B129">
         <v>292.67078600000002</v>
@@ -4697,7 +4698,7 @@
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B130">
         <v>292.83225099999999</v>
@@ -4708,7 +4709,7 @@
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B131">
         <v>292.102508</v>
@@ -4719,7 +4720,7 @@
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B132">
         <v>292.82086099999998</v>
@@ -4730,7 +4731,7 @@
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B133">
         <v>294.14280100000002</v>
@@ -4741,7 +4742,7 @@
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B134">
         <v>267.54444000000001</v>
@@ -4752,7 +4753,7 @@
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B135">
         <v>266.25499200000002</v>
@@ -4763,7 +4764,7 @@
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B136">
         <v>282.82444400000003</v>
@@ -4774,7 +4775,7 @@
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B137">
         <v>252.418308</v>
@@ -4785,7 +4786,7 @@
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B138">
         <v>253.064334</v>
@@ -4796,7 +4797,7 @@
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B139">
         <v>226.43700899999999</v>
@@ -4807,7 +4808,7 @@
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B140">
         <v>226.09825000000001</v>
@@ -4818,7 +4819,7 @@
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B141">
         <v>224.07482200000001</v>
@@ -4829,7 +4830,7 @@
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B142">
         <v>216.114001</v>
@@ -4840,7 +4841,7 @@
     </row>
     <row r="143" spans="1:3">
       <c r="A143" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B143">
         <v>32.670872000000003</v>
@@ -4851,7 +4852,7 @@
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B144">
         <v>207.28956299999999</v>
@@ -4860,9 +4861,9 @@
         <v>17.686458999999999</v>
       </c>
     </row>
-    <row r="145" spans="1:4">
+    <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B145">
         <v>193.91333800000001</v>
@@ -4871,9 +4872,9 @@
         <v>16.647044999999999</v>
       </c>
     </row>
-    <row r="146" spans="1:4">
+    <row r="146" spans="1:3">
       <c r="A146" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B146">
         <v>193.989812</v>
@@ -4882,9 +4883,9 @@
         <v>16.479883000000001</v>
       </c>
     </row>
-    <row r="147" spans="1:4">
+    <row r="147" spans="1:3">
       <c r="A147" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B147">
         <v>93.472650000000002</v>
@@ -4893,9 +4894,9 @@
         <v>7.9666680000000003</v>
       </c>
     </row>
-    <row r="148" spans="1:4">
+    <row r="148" spans="1:3">
       <c r="A148" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B148">
         <v>83.390383999999997</v>
@@ -4904,37 +4905,31 @@
         <v>7.07463</v>
       </c>
     </row>
-    <row r="149" spans="1:4">
+    <row r="149" spans="1:3">
       <c r="A149" t="s">
-        <v>71</v>
-      </c>
-      <c r="B149" t="s">
-        <v>3</v>
+        <v>70</v>
+      </c>
+      <c r="B149">
+        <v>200.76282800000001</v>
       </c>
       <c r="C149">
-        <v>200.76282800000001</v>
-      </c>
-      <c r="D149">
         <v>17.15869</v>
       </c>
     </row>
-    <row r="150" spans="1:4">
+    <row r="150" spans="1:3">
       <c r="A150" t="s">
-        <v>71</v>
-      </c>
-      <c r="B150" t="s">
-        <v>3</v>
+        <v>70</v>
+      </c>
+      <c r="B150">
+        <v>201.17855900000001</v>
       </c>
       <c r="C150">
-        <v>201.17855900000001</v>
-      </c>
-      <c r="D150">
         <v>17.142101</v>
       </c>
     </row>
-    <row r="151" spans="1:4">
+    <row r="151" spans="1:3">
       <c r="A151" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B151">
         <v>83.545385999999993</v>
@@ -4943,9 +4938,9 @@
         <v>7.1090679999999997</v>
       </c>
     </row>
-    <row r="152" spans="1:4">
+    <row r="152" spans="1:3">
       <c r="A152" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B152">
         <v>94.247737000000001</v>
@@ -4954,9 +4949,9 @@
         <v>7.94414</v>
       </c>
     </row>
-    <row r="153" spans="1:4">
+    <row r="153" spans="1:3">
       <c r="A153" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B153">
         <v>193.72072800000001</v>
@@ -4965,9 +4960,9 @@
         <v>16.424931000000001</v>
       </c>
     </row>
-    <row r="154" spans="1:4">
+    <row r="154" spans="1:3">
       <c r="A154" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B154">
         <v>192.775565</v>
@@ -4976,9 +4971,9 @@
         <v>16.110523000000001</v>
       </c>
     </row>
-    <row r="155" spans="1:4">
+    <row r="155" spans="1:3">
       <c r="A155" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B155">
         <v>207.29132200000001</v>
@@ -4987,9 +4982,9 @@
         <v>17.632891999999998</v>
       </c>
     </row>
-    <row r="156" spans="1:4">
+    <row r="156" spans="1:3">
       <c r="A156" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B156">
         <v>32.651131999999997</v>
@@ -4998,9 +4993,9 @@
         <v>2.7506360000000001</v>
       </c>
     </row>
-    <row r="157" spans="1:4">
+    <row r="157" spans="1:3">
       <c r="A157" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B157">
         <v>500</v>
@@ -5009,9 +5004,9 @@
         <v>18.266385</v>
       </c>
     </row>
-    <row r="158" spans="1:4">
+    <row r="158" spans="1:3">
       <c r="A158" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B158">
         <v>299.23320000000001</v>
@@ -5020,9 +5015,9 @@
         <v>19.108445</v>
       </c>
     </row>
-    <row r="159" spans="1:4">
+    <row r="159" spans="1:3">
       <c r="A159" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B159">
         <v>244.857426</v>
@@ -5031,9 +5026,9 @@
         <v>19.131243999999999</v>
       </c>
     </row>
-    <row r="160" spans="1:4">
+    <row r="160" spans="1:3">
       <c r="A160" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B160">
         <v>272.65515699999997</v>
@@ -5044,7 +5039,7 @@
     </row>
     <row r="161" spans="1:3">
       <c r="A161" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B161">
         <v>248.68656300000001</v>
@@ -5055,7 +5050,7 @@
     </row>
     <row r="162" spans="1:3">
       <c r="A162" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B162">
         <v>248.83504500000001</v>
@@ -5066,7 +5061,7 @@
     </row>
     <row r="163" spans="1:3">
       <c r="A163" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B163">
         <v>276.81735500000002</v>
@@ -5077,7 +5072,7 @@
     </row>
     <row r="164" spans="1:3">
       <c r="A164" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B164">
         <v>260.67281500000001</v>
@@ -5088,7 +5083,7 @@
     </row>
     <row r="165" spans="1:3">
       <c r="A165" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B165">
         <v>311.62367799999998</v>
@@ -5099,7 +5094,7 @@
     </row>
     <row r="166" spans="1:3">
       <c r="A166" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B166">
         <v>417.160211</v>
@@ -5110,7 +5105,7 @@
     </row>
     <row r="167" spans="1:3">
       <c r="A167" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B167">
         <v>361.62694800000003</v>
@@ -5121,7 +5116,7 @@
     </row>
     <row r="168" spans="1:3">
       <c r="A168" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B168">
         <v>336.03155199999998</v>
@@ -5132,7 +5127,7 @@
     </row>
     <row r="169" spans="1:3">
       <c r="A169" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B169">
         <v>325.27978100000001</v>
@@ -5143,7 +5138,7 @@
     </row>
     <row r="170" spans="1:3">
       <c r="A170" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B170">
         <v>294.498538</v>
@@ -5154,7 +5149,7 @@
     </row>
     <row r="171" spans="1:3">
       <c r="A171" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B171">
         <v>309.93006600000001</v>
@@ -5165,7 +5160,7 @@
     </row>
     <row r="172" spans="1:3">
       <c r="A172" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B172">
         <v>306.46525800000001</v>
@@ -5176,7 +5171,7 @@
     </row>
     <row r="173" spans="1:3">
       <c r="A173" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B173">
         <v>276.35902700000003</v>
@@ -5187,7 +5182,7 @@
     </row>
     <row r="174" spans="1:3">
       <c r="A174" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B174">
         <v>264.436037</v>
@@ -5198,7 +5193,7 @@
     </row>
     <row r="175" spans="1:3">
       <c r="A175" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B175">
         <v>10.990325</v>
@@ -5209,7 +5204,7 @@
     </row>
     <row r="176" spans="1:3">
       <c r="A176" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B176">
         <v>10.955360000000001</v>
@@ -5220,7 +5215,7 @@
     </row>
     <row r="177" spans="1:3">
       <c r="A177" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B177">
         <v>34.372168000000002</v>
@@ -5231,7 +5226,7 @@
     </row>
     <row r="178" spans="1:3">
       <c r="A178" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B178">
         <v>36.711027999999999</v>
@@ -5242,7 +5237,7 @@
     </row>
     <row r="179" spans="1:3">
       <c r="A179" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B179">
         <v>212.65095099999999</v>
@@ -5253,7 +5248,7 @@
     </row>
     <row r="180" spans="1:3">
       <c r="A180" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B180">
         <v>42.512566999999997</v>
@@ -5264,7 +5259,7 @@
     </row>
     <row r="181" spans="1:3">
       <c r="A181" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B181">
         <v>39.670209</v>
@@ -5275,7 +5270,7 @@
     </row>
     <row r="182" spans="1:3">
       <c r="A182" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B182">
         <v>317.32763599999998</v>
@@ -5286,7 +5281,7 @@
     </row>
     <row r="183" spans="1:3">
       <c r="A183" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B183">
         <v>337.16993200000002</v>
@@ -5297,7 +5292,7 @@
     </row>
     <row r="184" spans="1:3">
       <c r="A184" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B184">
         <v>350.66914500000001</v>
@@ -5308,7 +5303,7 @@
     </row>
     <row r="185" spans="1:3">
       <c r="A185" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B185">
         <v>180.29478599999999</v>
@@ -5319,7 +5314,7 @@
     </row>
     <row r="186" spans="1:3">
       <c r="A186" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B186">
         <v>298.73103600000002</v>
@@ -5330,7 +5325,7 @@
     </row>
     <row r="187" spans="1:3">
       <c r="A187" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B187">
         <v>301.46888300000001</v>
@@ -5341,7 +5336,7 @@
     </row>
     <row r="188" spans="1:3">
       <c r="A188" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B188">
         <v>302.641592</v>
@@ -5352,7 +5347,7 @@
     </row>
     <row r="189" spans="1:3">
       <c r="A189" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B189">
         <v>307.19630599999999</v>
@@ -5363,7 +5358,7 @@
     </row>
     <row r="190" spans="1:3">
       <c r="A190" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B190">
         <v>180.601168</v>
@@ -5374,7 +5369,7 @@
     </row>
     <row r="191" spans="1:3">
       <c r="A191" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B191">
         <v>282.66567400000002</v>
@@ -5385,7 +5380,7 @@
     </row>
     <row r="192" spans="1:3">
       <c r="A192" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B192">
         <v>283.27106099999997</v>
@@ -5396,7 +5391,7 @@
     </row>
     <row r="193" spans="1:3">
       <c r="A193" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B193">
         <v>283.67868600000003</v>
@@ -5407,7 +5402,7 @@
     </row>
     <row r="194" spans="1:3">
       <c r="A194" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B194">
         <v>282.87317000000002</v>
@@ -5418,7 +5413,7 @@
     </row>
     <row r="195" spans="1:3">
       <c r="A195" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B195">
         <v>285.05495400000001</v>
@@ -5429,7 +5424,7 @@
     </row>
     <row r="196" spans="1:3">
       <c r="A196" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B196">
         <v>284.86199499999998</v>
@@ -5440,7 +5435,7 @@
     </row>
     <row r="197" spans="1:3">
       <c r="A197" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B197">
         <v>179.79143300000001</v>
@@ -5451,7 +5446,7 @@
     </row>
     <row r="198" spans="1:3">
       <c r="A198" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B198">
         <v>284.72751399999999</v>
@@ -5462,7 +5457,7 @@
     </row>
     <row r="199" spans="1:3">
       <c r="A199" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B199">
         <v>284.27877100000001</v>
@@ -5473,7 +5468,7 @@
     </row>
     <row r="200" spans="1:3">
       <c r="A200" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B200">
         <v>284.15458799999999</v>

</xml_diff>